<commit_message>
Added retest stroop data enkavi
+ code to reformat enkavi stroop dataset
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C307BF-982C-418A-923F-41C6DE2F4E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B75B16-1C64-43D2-A26D-922FBFCF5077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="381">
   <si>
     <t>study</t>
   </si>
@@ -1131,6 +1131,57 @@
   </si>
   <si>
     <t>Univeristy of Virginia</t>
+  </si>
+  <si>
+    <t>Enkavi</t>
+  </si>
+  <si>
+    <t>A. Zeynep Enkavia, Ian W. Eisenberg, Patrick G. Bissett, Gina L. Mazza, David P. MacKinnon, Lisa A. Marsc, Russell A. Poldrack</t>
+  </si>
+  <si>
+    <t>zenkavi@stanford.edu</t>
+  </si>
+  <si>
+    <t>self regulation, retest reliability, individual differences</t>
+  </si>
+  <si>
+    <t>enkavi_2019_large</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Large-scale investigation into retest-reliabilities of self-regulation measures based on a) a literature review of reported reliability measures and b) newly collected data of the same task battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partipants recruited on Mturk </t>
+  </si>
+  <si>
+    <t>Enkavi stroop</t>
+  </si>
+  <si>
+    <t>Enkavi simon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simon </t>
+  </si>
+  <si>
+    <t>Color stroop task: Participants categorized the color of a presented word using one of three keys; irrelevant stimulus was the words' semantic meaning</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/jstbcs/acdc-database/main/data/enkavi_2019_large/stroop.csv</t>
+  </si>
+  <si>
+    <t>Enkavi stroop wave 1</t>
+  </si>
+  <si>
+    <t>Enkavi stroop wave 2</t>
+  </si>
+  <si>
+    <t>Test phase; first measurement wave (July - September 2016)</t>
+  </si>
+  <si>
+    <t>Retest phase; 2nd measurement wave (November 2016 - March 2017)</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1203,6 +1254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1220,7 +1277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1234,6 +1291,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1549,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1823,6 +1881,32 @@
         <v>67</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C11">
+        <v>2019</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="G11" t="s">
+        <v>367</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="I11" t="s">
+        <v>368</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{EEA56B93-BF73-4856-9DA1-9A3B5BA67A8B}"/>
@@ -1833,6 +1917,7 @@
     <hyperlink ref="F7" r:id="rId6" xr:uid="{86228BAE-DDA4-4767-90AD-EC51F2564A28}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{2AC655EA-B2E6-46BA-9AF5-7CF2241941BD}"/>
     <hyperlink ref="F5" r:id="rId8" xr:uid="{1AC344C5-7FEF-42ED-A7EA-742769BFDA83}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{6EE7083C-CB23-46FC-B9FB-ED39AD2DCC15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1840,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2330,6 +2415,18 @@
         <v>90</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>364</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" t="s">
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2339,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CF0719-54A4-4A0C-BDDA-03EA16BD7F02}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3189,6 +3286,26 @@
         <v>349</v>
       </c>
     </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>364</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>34.1</v>
+      </c>
+      <c r="E36">
+        <v>0.52</v>
+      </c>
+      <c r="F36" s="11">
+        <v>150</v>
+      </c>
+      <c r="G36" t="s">
+        <v>371</v>
+      </c>
+    </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.35">
       <c r="S42" s="10"/>
     </row>
@@ -3220,10 +3337,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3663,6 +3780,31 @@
         <v>162</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>372</v>
+      </c>
+      <c r="C32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>373</v>
+      </c>
+      <c r="C33" t="s">
+        <v>374</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3670,10 +3812,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5496,6 +5638,41 @@
       </c>
       <c r="K51" t="s">
         <v>285</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>372</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52">
+        <v>150</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>96</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>103</v>
+      </c>
+      <c r="I52" t="s">
+        <v>175</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="K52" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -5549,6 +5726,7 @@
     <hyperlink ref="J10" r:id="rId47" xr:uid="{20972848-216D-4D3D-983A-1819FA93E846}"/>
     <hyperlink ref="J13" r:id="rId48" xr:uid="{6FCCDE21-475D-492D-9C7D-8755A92556BE}"/>
     <hyperlink ref="J12" r:id="rId49" xr:uid="{BE262AB6-BEC1-4DDB-B754-32D92F1510FD}"/>
+    <hyperlink ref="J52" r:id="rId50" xr:uid="{02E21F3F-A79D-4E4D-B123-FB6E9F80DD62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5556,10 +5734,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6516,6 +6694,34 @@
         <v>289</v>
       </c>
     </row>
+    <row r="69" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>377</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>378</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6523,10 +6729,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7132,6 +7338,14 @@
         <v>284</v>
       </c>
     </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>372</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add enkavi simon retest data
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B75B16-1C64-43D2-A26D-922FBFCF5077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359A3687-835C-4B79-B880-96B223179D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="386">
   <si>
     <t>study</t>
   </si>
@@ -1182,6 +1182,21 @@
   </si>
   <si>
     <t>Retest phase; 2nd measurement wave (November 2016 - March 2017)</t>
+  </si>
+  <si>
+    <t>Participants had to identify the color of a box (relevant stimulus) which appeared to the left or right side of the screen (location: irrelevant stimulus) by pressing a LEFT or RIGHT arrow on a computer keyboard. In congruent trials the location of the target word matched the response key; in incongruent trials it did not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no info </t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/jstbcs/acdc-database/main/data/enkavi_2019_large/simon.csv</t>
+  </si>
+  <si>
+    <t>dataset51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkavi simon </t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1292,6 +1307,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1927,7 +1943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -2436,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CF0719-54A4-4A0C-BDDA-03EA16BD7F02}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3299,8 +3315,8 @@
       <c r="E36">
         <v>0.52</v>
       </c>
-      <c r="F36" s="11">
-        <v>150</v>
+      <c r="F36" s="12">
+        <v>522</v>
       </c>
       <c r="G36" t="s">
         <v>371</v>
@@ -3339,8 +3355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3794,7 +3810,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3803,6 +3819,9 @@
       </c>
       <c r="C33" t="s">
         <v>374</v>
+      </c>
+      <c r="D33" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3812,10 +3831,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V52"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5651,7 +5670,7 @@
         <v>103</v>
       </c>
       <c r="D52">
-        <v>150</v>
+        <v>522</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -5672,7 +5691,42 @@
         <v>376</v>
       </c>
       <c r="K52" t="s">
-        <v>215</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>373</v>
+      </c>
+      <c r="C53" t="s">
+        <v>382</v>
+      </c>
+      <c r="D53">
+        <v>522</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>100</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53" t="s">
+        <v>103</v>
+      </c>
+      <c r="I53" t="s">
+        <v>175</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="K53" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -5727,6 +5781,7 @@
     <hyperlink ref="J13" r:id="rId48" xr:uid="{6FCCDE21-475D-492D-9C7D-8755A92556BE}"/>
     <hyperlink ref="J12" r:id="rId49" xr:uid="{BE262AB6-BEC1-4DDB-B754-32D92F1510FD}"/>
     <hyperlink ref="J52" r:id="rId50" xr:uid="{02E21F3F-A79D-4E4D-B123-FB6E9F80DD62}"/>
+    <hyperlink ref="J53" r:id="rId51" xr:uid="{DEE600D3-A019-46D1-9DC3-9A6FDEE878D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5734,10 +5789,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6722,6 +6777,14 @@
         <v>380</v>
       </c>
     </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>385</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6729,10 +6792,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7346,6 +7409,14 @@
         <v>372</v>
       </c>
     </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created list object for Enkavi et al data
+ new rows in Book excel
+ script to replicate list object
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359A3687-835C-4B79-B880-96B223179D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AB5628-CB58-4AA8-9C21-96ACE656D061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="388">
   <si>
     <t>study</t>
   </si>
@@ -1136,9 +1136,6 @@
     <t>Enkavi</t>
   </si>
   <si>
-    <t>A. Zeynep Enkavia, Ian W. Eisenberg, Patrick G. Bissett, Gina L. Mazza, David P. MacKinnon, Lisa A. Marsc, Russell A. Poldrack</t>
-  </si>
-  <si>
     <t>zenkavi@stanford.edu</t>
   </si>
   <si>
@@ -1148,9 +1145,6 @@
     <t>enkavi_2019_large</t>
   </si>
   <si>
-    <t>!</t>
-  </si>
-  <si>
     <t>Large-scale investigation into retest-reliabilities of self-regulation measures based on a) a literature review of reported reliability measures and b) newly collected data of the same task battery</t>
   </si>
   <si>
@@ -1196,7 +1190,19 @@
     <t>dataset51</t>
   </si>
   <si>
-    <t xml:space="preserve">Enkavi simon </t>
+    <t>Enkavi simon wave 1</t>
+  </si>
+  <si>
+    <t>Enkavi simon wave 2</t>
+  </si>
+  <si>
+    <t>Enkavi, A. Z., Eisenberg, I. W., Bissett, P. G., Mazza, G. L., MacKinnon, D. P., Marsch, L. A., &amp; Poldrack, R. A. (2019). Large-scale analysis of test–retest reliabilities of self-regulation measures. Proceedings of the National Academy of Sciences of the National Academy of Sciences of the United States of America, 116(12), 5472–5477. https://doi.org/10.1073/pnas.1818430116</t>
+  </si>
+  <si>
+    <t>A. Zeynep Enkavi, Ian W. Eisenberg, Patrick G. Bissett, Gina L. Mazza, David P. MacKinnon, Lisa A. Marsc, Russell A. Poldrack</t>
+  </si>
+  <si>
+    <t>dataset52</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1269,12 +1275,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,7 +1292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1306,7 +1306,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1626,7 +1625,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1902,7 +1901,7 @@
         <v>364</v>
       </c>
       <c r="B11" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
       <c r="C11">
         <v>2019</v>
@@ -1911,16 +1910,16 @@
         <v>32</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G11" t="s">
         <v>366</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>385</v>
+      </c>
+      <c r="I11" t="s">
         <v>367</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="I11" t="s">
-        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -1943,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2438,9 +2437,11 @@
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="11"/>
+      <c r="C35" s="11">
+        <v>35</v>
+      </c>
       <c r="D35" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -3315,11 +3316,11 @@
       <c r="E36">
         <v>0.52</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36">
         <v>522</v>
       </c>
       <c r="G36" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.35">
@@ -3355,8 +3356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3801,13 +3802,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C32" t="s">
         <v>117</v>
       </c>
       <c r="D32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -3815,13 +3816,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C33" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D33" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -3834,7 +3835,7 @@
   <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5664,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C52" t="s">
         <v>103</v>
@@ -5688,10 +5689,10 @@
         <v>175</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K52" t="s">
-        <v>202</v>
+        <v>382</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
@@ -5699,10 +5700,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C53" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D53">
         <v>522</v>
@@ -5723,10 +5724,10 @@
         <v>175</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K53" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -5789,10 +5790,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6754,13 +6755,13 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
+        <v>375</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>377</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6768,21 +6769,41 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C70">
         <v>2</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>385</v>
+        <v>383</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>384</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -6792,10 +6813,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7406,7 +7427,7 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -7414,7 +7435,31 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>373</v>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code and excel entries to create kucina list
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AB5628-CB58-4AA8-9C21-96ACE656D061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5F441-8F8C-451B-A642-8A12AFD4EB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="446">
   <si>
     <t>study</t>
   </si>
@@ -1203,6 +1203,181 @@
   </si>
   <si>
     <t>dataset52</t>
+  </si>
+  <si>
+    <t>Kucina</t>
+  </si>
+  <si>
+    <t>Talira Kucina, Lindsay Wells, Ian Lewis, Kristy de Salas, Amelia Kohl, Matthew A. Palmer, James D. Sauer, Dora Matzke, Eugene Aidman &amp; Andrew Heathcote</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>talira.kucina@utas.edu.au</t>
+  </si>
+  <si>
+    <t>attentional control, individual differences, reliability paradox</t>
+  </si>
+  <si>
+    <t>kucina_2023_calibration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kucina </t>
+  </si>
+  <si>
+    <t>Kucina 1</t>
+  </si>
+  <si>
+    <t>Kucina 2</t>
+  </si>
+  <si>
+    <t>Kucina 3</t>
+  </si>
+  <si>
+    <t>Kucina 4</t>
+  </si>
+  <si>
+    <t>Kucina 5</t>
+  </si>
+  <si>
+    <t>Participants completing a traditional flanker task ("Flanker1")</t>
+  </si>
+  <si>
+    <t>Participants completing a flanker task with additional manipulation ("Flanker2")</t>
+  </si>
+  <si>
+    <t>Participants completing a stroop task with additional manipulation ("Stroop2")</t>
+  </si>
+  <si>
+    <t>Participants completing a simon task with additional manipulation ("Simon2")</t>
+  </si>
+  <si>
+    <t>Participants completing a combination of stroop and simon task with no additional manipulation ("Stroopon")</t>
+  </si>
+  <si>
+    <t>Participants completing a combination of stroop and simon task with additional manipulation ("Stroopon2")</t>
+  </si>
+  <si>
+    <t>Kucina Stroop2</t>
+  </si>
+  <si>
+    <t>Kucina Simon2</t>
+  </si>
+  <si>
+    <t>Kucina Stroopon</t>
+  </si>
+  <si>
+    <t>Kucina Stroopon2</t>
+  </si>
+  <si>
+    <t>Kucina Flanker1</t>
+  </si>
+  <si>
+    <t>Kucina Flanker2</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Introduction of gamified and calibrated versions of stroop, simon, and flanker tasks with an additional manipulation to encourage processing of conflicting information,
+as a combination of stroop+simon task in order to enhance the reliability of estimations of individual differences in attentional control.</t>
+  </si>
+  <si>
+    <t>Participants had to identify the color of a rectangle (either orange associated with a right key response and blue with a left key, or vice versa); irrelevant stimulus was the location the rectangle appeared in (either right or left side of the screen); In a randomly chosen 1/3 of the trials, participants were asked to provide a second response afterwards, indicating the actual location of the rectangle (i.e., the irrelevant stimulus)</t>
+  </si>
+  <si>
+    <t>Classical stroop task with a modfication: Participants had to identify the font color words while ignoring their semantic meaning; however in 1/3 of the trials they were asked to additionally provide a second response indicating the irrelevant stimulus they previously had to surpress (i.e., semantic meaning of the word)</t>
+  </si>
+  <si>
+    <t>A combination of simon and stroop task: Color words (blue or orange) in colored font (blue or orange) appeared either on the left or right side of the screen. Participants had to identify font color by pressing a lkey with their right (/) or left (Z) hand.Irrelevant stimuli were semantic word meaning and the side the word appeared on. Trials could be either double-congruent (font color was in line with both semantic meaning and the correct response key was on the same side as the word's location on the screen) or double-incongruent (font color did not correspond to the word's meaning and the word appeared on the other side of the screen than the correct key response)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A combination of simon and stroop task: Color words (blue or orange) in colored font (blue or orange) appeared either on the left or right side of the screen. Participants had to identify font color by pressing a lkey with their right (/) or left (Z) hand.Irrelevant stimuli were semantic word meaning and the side the word appeared on. Trials could be either double-congruent (font color was in line with both semantic meaning and the correct response key was on the same side as the word's location on the screen) or double-incongruent (font color did not correspond to the word's meaning and the word appeared on the other side of the screen than the correct key response); Additionally, in a randomly chosen 1/3 of the trials, participants were asked to additionally provide a second response after the first in which they had to indicate one of the irrevelant stimuli (i.e., either the semantic meaning of the word or its location) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrow flanker task: Participants had to identify the direction of the central arrow (left or right); irrelevant stimulus was the direction of the four flanking arrows; the central arrow's location on the screen appeared slightly deviated from the center of the screen in some trials to introduce spatial uncertainty; responses were given by pressing Z with the left hand or / with the right hand for left and right responses respectively </t>
+  </si>
+  <si>
+    <t>Arrow flanker task with a modification: Participants had to identify the direction of the central arrow (left or right); irrelevant stimulus was the direction of the four flanking arrows; the central arrow's location on the screen appeared slightly deviated from the center of the screen in some trials to introduce spatial uncertainty; responses were given by pressing Z with the left hand or / with the right hand for left and right responses respectively. However on a randomly chosen 33.33% of the trials participants were asked to provide an additional second response after the first in which they had to indicate the irrelevant stimulus (i.e., the direction of the flanking arrows)</t>
+  </si>
+  <si>
+    <t>excluded participants with incomplete data and those who failed a tutorial at the start of the experiment</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/jstbcs/acdc-database/main/data/kucina_2023_calibration/data4.csv</t>
+  </si>
+  <si>
+    <t>dataset53</t>
+  </si>
+  <si>
+    <t>dataset54</t>
+  </si>
+  <si>
+    <t>dataset55</t>
+  </si>
+  <si>
+    <t>dataset56</t>
+  </si>
+  <si>
+    <t>dataset57</t>
+  </si>
+  <si>
+    <t>dataset58</t>
+  </si>
+  <si>
+    <t>none but "hurry up" message after 2 sec</t>
+  </si>
+  <si>
+    <t>Kucina Stroop2- Single response trial</t>
+  </si>
+  <si>
+    <t>Kucina Simon2- Single response trial</t>
+  </si>
+  <si>
+    <t>Kucina Stroop2- Double response trial</t>
+  </si>
+  <si>
+    <t>Kucina Simon2- Double response trial</t>
+  </si>
+  <si>
+    <t>No within manipulation</t>
+  </si>
+  <si>
+    <t>Kucina Stroopon2 - Single response trial</t>
+  </si>
+  <si>
+    <t>Kucina Stroopon2 - Double response trial</t>
+  </si>
+  <si>
+    <t>Single response trial: Trials on which articipants had to respond to the relevant stimulus only (font color)</t>
+  </si>
+  <si>
+    <t>Single response trial: Trials on which articipants had to respond to the relevant stimulus only (rectangle color)</t>
+  </si>
+  <si>
+    <t>Double response trial: Trials on which participants first responded to the relevant stimulus (font color) and where then asked to additionally respond to the irrelevant stimulus afterwards (semantic meaning of word)</t>
+  </si>
+  <si>
+    <t>Double response trial: Trials on which participants first responded to the relevant stimulus (color of rectangle) and where then asked to additionally respond to the irrelevant stimulus afterwards (side the rectangle appeared on)</t>
+  </si>
+  <si>
+    <t>Double response trial: Trials on which participants first responded to the relevant stimulus (font color) and where then asked to additionally respond to the irrelevant stimulus afterwards (semantic meaning of word// side of screen the word appeared on)</t>
+  </si>
+  <si>
+    <t>Kucina Flanker2- Single response trial</t>
+  </si>
+  <si>
+    <t>Kucina Flanker2- Double response trial</t>
+  </si>
+  <si>
+    <t>Single response trial: Trials on which articipants had to respond to the relevant stimulus only (direction of central arrow)</t>
+  </si>
+  <si>
+    <t>Double response trial: Trials on which participants first responded to the relevant stimulus (direction of central arrow) and where then asked to additionally respond to the irrelevant stimulus afterwards (direction of flanking arrows)</t>
+  </si>
+  <si>
+    <t>Kucina 6</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1275,6 +1450,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,7 +1473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1306,7 +1487,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1622,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1922,6 +2106,32 @@
         <v>367</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" t="s">
+        <v>389</v>
+      </c>
+      <c r="C12">
+        <v>2023</v>
+      </c>
+      <c r="E12" t="s">
+        <v>390</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G12" t="s">
+        <v>392</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" t="s">
+        <v>393</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{EEA56B93-BF73-4856-9DA1-9A3B5BA67A8B}"/>
@@ -1933,6 +2143,7 @@
     <hyperlink ref="F8" r:id="rId7" xr:uid="{2AC655EA-B2E6-46BA-9AF5-7CF2241941BD}"/>
     <hyperlink ref="F5" r:id="rId8" xr:uid="{1AC344C5-7FEF-42ED-A7EA-742769BFDA83}"/>
     <hyperlink ref="F11" r:id="rId9" xr:uid="{6EE7083C-CB23-46FC-B9FB-ED39AD2DCC15}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{E1360CE3-FFB6-477F-A262-E234B0E97B60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1940,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2437,11 +2648,25 @@
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35">
         <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>394</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -2453,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CF0719-54A4-4A0C-BDDA-03EA16BD7F02}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2467,7 +2692,7 @@
     <col min="7" max="7" width="27.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>91</v>
       </c>
@@ -2490,7 +2715,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2507,7 +2732,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2524,7 +2749,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2548,7 +2773,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2572,7 +2797,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2596,7 +2821,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2620,7 +2845,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2644,7 +2869,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2661,7 +2886,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2678,7 +2903,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2695,7 +2920,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2719,7 +2944,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2742,7 +2967,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2763,7 +2988,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2785,14 +3010,16 @@
       <c r="G15" t="s">
         <v>98</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="K15">
+      <c r="J15" s="10"/>
+      <c r="K15" s="10">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>246</v>
       </c>
@@ -2811,14 +3038,16 @@
       <c r="G16" t="s">
         <v>98</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="K16">
+      <c r="J16" s="10"/>
+      <c r="K16" s="10">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>248</v>
       </c>
@@ -2837,14 +3066,16 @@
       <c r="G17" t="s">
         <v>98</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="K17">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>250</v>
       </c>
@@ -2863,14 +3094,16 @@
       <c r="G18" t="s">
         <v>98</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="K18">
+      <c r="J18" s="10"/>
+      <c r="K18" s="10">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>252</v>
       </c>
@@ -2889,14 +3122,16 @@
       <c r="G19" t="s">
         <v>98</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="K19">
+      <c r="J19" s="10"/>
+      <c r="K19" s="10">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>254</v>
       </c>
@@ -2915,14 +3150,16 @@
       <c r="G20" t="s">
         <v>98</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="K20">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>256</v>
       </c>
@@ -2941,14 +3178,16 @@
       <c r="G21" t="s">
         <v>98</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="K21">
+      <c r="J21" s="10"/>
+      <c r="K21" s="10">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>258</v>
       </c>
@@ -2967,14 +3206,16 @@
       <c r="G22" t="s">
         <v>98</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="K22">
+      <c r="J22" s="10"/>
+      <c r="K22" s="10">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>260</v>
       </c>
@@ -2993,14 +3234,16 @@
       <c r="G23" t="s">
         <v>98</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="K23">
+      <c r="J23" s="10"/>
+      <c r="K23" s="10">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>262</v>
       </c>
@@ -3019,14 +3262,16 @@
       <c r="G24" t="s">
         <v>354</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="K24">
+      <c r="J24" s="10"/>
+      <c r="K24" s="10">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>264</v>
       </c>
@@ -3045,14 +3290,16 @@
       <c r="G25" t="s">
         <v>98</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="K25">
+      <c r="J25" s="10"/>
+      <c r="K25" s="10">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>266</v>
       </c>
@@ -3071,14 +3318,16 @@
       <c r="G26" t="s">
         <v>98</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="K26">
+      <c r="J26" s="10"/>
+      <c r="K26" s="10">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>268</v>
       </c>
@@ -3097,14 +3346,16 @@
       <c r="G27" t="s">
         <v>98</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="K27">
+      <c r="J27" s="10"/>
+      <c r="K27" s="10">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>270</v>
       </c>
@@ -3123,14 +3374,16 @@
       <c r="G28" t="s">
         <v>98</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="K28">
+      <c r="J28" s="10"/>
+      <c r="K28" s="10">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>272</v>
       </c>
@@ -3149,11 +3402,14 @@
       <c r="G29" t="s">
         <v>357</v>
       </c>
-      <c r="K29">
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>274</v>
       </c>
@@ -3172,14 +3428,16 @@
       <c r="G30" t="s">
         <v>98</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="K30">
+      <c r="J30" s="10"/>
+      <c r="K30" s="10">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>276</v>
       </c>
@@ -3198,14 +3456,16 @@
       <c r="G31" t="s">
         <v>98</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="K31">
+      <c r="J31" s="10"/>
+      <c r="K31" s="10">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>278</v>
       </c>
@@ -3224,12 +3484,14 @@
       <c r="G32" t="s">
         <v>98</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="K32">
+      <c r="J32" s="10"/>
+      <c r="K32" s="10">
         <v>31</v>
       </c>
+      <c r="L32" s="10"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
@@ -3250,12 +3512,14 @@
       <c r="G33" t="s">
         <v>354</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="K33">
+      <c r="J33" s="10"/>
+      <c r="K33" s="10">
         <v>32</v>
       </c>
+      <c r="L33" s="10"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
@@ -3276,9 +3540,12 @@
       <c r="G34" t="s">
         <v>98</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="10" t="s">
         <v>362</v>
       </c>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
@@ -3299,9 +3566,12 @@
       <c r="G35" t="s">
         <v>98</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="10" t="s">
         <v>349</v>
       </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
@@ -3322,8 +3592,91 @@
       <c r="G36" t="s">
         <v>369</v>
       </c>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>395</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>396</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>31</v>
+      </c>
+      <c r="G38" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>397</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>398</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>31</v>
+      </c>
+      <c r="G40" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>399</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>33</v>
+      </c>
+      <c r="G41" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>445</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>401</v>
+      </c>
       <c r="S42" s="10"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.35">
@@ -3354,10 +3707,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3799,7 +4152,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
         <v>370</v>
@@ -3813,7 +4166,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
         <v>371</v>
@@ -3823,6 +4176,90 @@
       </c>
       <c r="D33" t="s">
         <v>379</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>406</v>
+      </c>
+      <c r="C34" t="s">
+        <v>412</v>
+      </c>
+      <c r="D34" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>407</v>
+      </c>
+      <c r="C35" t="s">
+        <v>412</v>
+      </c>
+      <c r="D35" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>408</v>
+      </c>
+      <c r="C36" t="s">
+        <v>412</v>
+      </c>
+      <c r="D36" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>409</v>
+      </c>
+      <c r="C37" t="s">
+        <v>412</v>
+      </c>
+      <c r="D37" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>410</v>
+      </c>
+      <c r="C38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>411</v>
+      </c>
+      <c r="C39" t="s">
+        <v>412</v>
+      </c>
+      <c r="D39" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -3832,10 +4269,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V53"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5728,6 +6165,223 @@
       </c>
       <c r="K53" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>406</v>
+      </c>
+      <c r="C56" t="s">
+        <v>420</v>
+      </c>
+      <c r="D56" t="s">
+        <v>104</v>
+      </c>
+      <c r="H56" t="s">
+        <v>103</v>
+      </c>
+      <c r="I56" t="s">
+        <v>428</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="K56" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>407</v>
+      </c>
+      <c r="C57" t="s">
+        <v>420</v>
+      </c>
+      <c r="D57">
+        <v>31</v>
+      </c>
+      <c r="E57">
+        <v>36</v>
+      </c>
+      <c r="F57">
+        <v>12</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" t="s">
+        <v>428</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="K57" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>408</v>
+      </c>
+      <c r="C58" t="s">
+        <v>420</v>
+      </c>
+      <c r="D58">
+        <v>30</v>
+      </c>
+      <c r="E58">
+        <v>36</v>
+      </c>
+      <c r="F58">
+        <v>12</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58" t="s">
+        <v>103</v>
+      </c>
+      <c r="I58" t="s">
+        <v>428</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="K58" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>409</v>
+      </c>
+      <c r="C59" t="s">
+        <v>420</v>
+      </c>
+      <c r="D59">
+        <v>31</v>
+      </c>
+      <c r="E59">
+        <v>36</v>
+      </c>
+      <c r="F59">
+        <v>12</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>103</v>
+      </c>
+      <c r="I59" t="s">
+        <v>428</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="K59" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>410</v>
+      </c>
+      <c r="C60" t="s">
+        <v>420</v>
+      </c>
+      <c r="D60">
+        <v>33</v>
+      </c>
+      <c r="E60">
+        <v>36</v>
+      </c>
+      <c r="F60">
+        <v>12</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I60" t="s">
+        <v>428</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="K60" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>411</v>
+      </c>
+      <c r="C61" t="s">
+        <v>420</v>
+      </c>
+      <c r="D61">
+        <v>30</v>
+      </c>
+      <c r="E61">
+        <v>36</v>
+      </c>
+      <c r="F61">
+        <v>12</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61" t="s">
+        <v>103</v>
+      </c>
+      <c r="I61" t="s">
+        <v>428</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="K61" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -5783,6 +6437,12 @@
     <hyperlink ref="J12" r:id="rId49" xr:uid="{BE262AB6-BEC1-4DDB-B754-32D92F1510FD}"/>
     <hyperlink ref="J52" r:id="rId50" xr:uid="{02E21F3F-A79D-4E4D-B123-FB6E9F80DD62}"/>
     <hyperlink ref="J53" r:id="rId51" xr:uid="{DEE600D3-A019-46D1-9DC3-9A6FDEE878D8}"/>
+    <hyperlink ref="J56" r:id="rId52" xr:uid="{008F5847-4465-49F8-9A77-1D744DA01444}"/>
+    <hyperlink ref="J57" r:id="rId53" xr:uid="{864E1D2E-A086-4BE7-82DF-794CE1732C9D}"/>
+    <hyperlink ref="J58" r:id="rId54" xr:uid="{4D65D99D-5735-4D4A-ACC3-857256C8639D}"/>
+    <hyperlink ref="J59" r:id="rId55" xr:uid="{CE4B6D3A-CEF7-44CB-AC73-740F7CFC5E01}"/>
+    <hyperlink ref="J60" r:id="rId56" xr:uid="{992FA71F-3DB4-4C96-AB9E-13D6BE604AAC}"/>
+    <hyperlink ref="J61" r:id="rId57" xr:uid="{DA7FE050-E207-4231-B433-4E90CAB92A1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5790,10 +6450,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6750,7 +7410,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1</v>
       </c>
@@ -6760,7 +7420,7 @@
       <c r="C69">
         <v>1</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" t="s">
         <v>377</v>
       </c>
     </row>
@@ -6774,11 +7434,11 @@
       <c r="C70">
         <v>2</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1</v>
       </c>
@@ -6788,11 +7448,11 @@
       <c r="C71">
         <v>1</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1</v>
       </c>
@@ -6802,8 +7462,118 @@
       <c r="C72">
         <v>2</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" t="s">
         <v>378</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>429</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>431</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>430</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>432</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>408</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>434</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>435</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>410</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>441</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>442</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -6813,10 +7583,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7358,7 +8128,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1</v>
       </c>
@@ -7366,7 +8136,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1</v>
       </c>
@@ -7374,7 +8144,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1</v>
       </c>
@@ -7382,7 +8152,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1</v>
       </c>
@@ -7390,7 +8160,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1</v>
       </c>
@@ -7398,7 +8168,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1</v>
       </c>
@@ -7406,7 +8176,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1</v>
       </c>
@@ -7414,7 +8184,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1</v>
       </c>
@@ -7422,7 +8192,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1</v>
       </c>
@@ -7430,7 +8200,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1</v>
       </c>
@@ -7438,7 +8208,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
@@ -7446,7 +8216,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1</v>
       </c>
@@ -7454,12 +8224,208 @@
         <v>383</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1</v>
       </c>
       <c r="B77" t="s">
         <v>384</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="C78" s="12">
+        <v>1</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="C79" s="12">
+        <v>2</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C80" s="12">
+        <v>1</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="C81" s="12">
+        <v>2</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>3</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="C82" s="12">
+        <v>1</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="C83" s="12">
+        <v>2</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C84" s="12">
+        <v>1</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="C85" s="12">
+        <v>2</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="C86" s="12">
+        <v>1</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="C87" s="12">
+        <v>1</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="C88" s="12">
+        <v>2</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="C89" s="12">
+        <v>1</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>3</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="C90" s="12">
+        <v>1</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>3</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="C91" s="12">
+        <v>2</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated reymermet and created kucina data
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5F441-8F8C-451B-A642-8A12AFD4EB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF1DEBB-2CC5-4A9C-8DDB-3475C732F655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2679,7 +2679,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="B37" sqref="B37:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7585,7 +7585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
       <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to kucina_list and shiny
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF1DEBB-2CC5-4A9C-8DDB-3475C732F655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D9162-31C2-498C-8E10-F24A3236A593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="447">
   <si>
     <t>study</t>
   </si>
@@ -1378,6 +1378,9 @@
   </si>
   <si>
     <t>Kucina 6</t>
+  </si>
+  <si>
+    <t>Kucina, T., Wells, L., Lewis, I., De Salas, K., Kohl, A., Palmer, M. A., Sauer, J. D., Matzke, D., Aidman, E., &amp; Heathcote, A. (2023). Calibration of cognitive tests to address the reliability paradox for decision-conflict tasks. Nature Communications, 14(1). https://doi.org/10.1038/s41467-023-37777-2</t>
   </si>
 </sst>
 </file>
@@ -1440,7 +1443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1450,12 +1453,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1487,9 +1484,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1808,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2125,8 +2124,8 @@
       <c r="G12" t="s">
         <v>392</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>104</v>
+      <c r="H12" s="12" t="s">
+        <v>446</v>
       </c>
       <c r="I12" t="s">
         <v>393</v>
@@ -7585,7 +7584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
@@ -8236,13 +8235,13 @@
       <c r="A78">
         <v>3</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="C78" s="12">
-        <v>1</v>
-      </c>
-      <c r="D78" s="12" t="s">
+      <c r="C78" s="11">
+        <v>1</v>
+      </c>
+      <c r="D78" s="11" t="s">
         <v>377</v>
       </c>
     </row>
@@ -8250,13 +8249,13 @@
       <c r="A79">
         <v>3</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C79" s="12">
+      <c r="C79" s="11">
         <v>2</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="11" t="s">
         <v>378</v>
       </c>
     </row>
@@ -8264,13 +8263,13 @@
       <c r="A80">
         <v>3</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="C80" s="12">
-        <v>1</v>
-      </c>
-      <c r="D80" s="12" t="s">
+      <c r="C80" s="11">
+        <v>1</v>
+      </c>
+      <c r="D80" s="11" t="s">
         <v>377</v>
       </c>
     </row>
@@ -8278,13 +8277,13 @@
       <c r="A81">
         <v>3</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="C81" s="12">
+      <c r="C81" s="11">
         <v>2</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="11" t="s">
         <v>378</v>
       </c>
     </row>
@@ -8292,13 +8291,13 @@
       <c r="A82">
         <v>3</v>
       </c>
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="C82" s="12">
-        <v>1</v>
-      </c>
-      <c r="D82" s="12" t="s">
+      <c r="C82" s="11">
+        <v>1</v>
+      </c>
+      <c r="D82" s="11" t="s">
         <v>436</v>
       </c>
     </row>
@@ -8306,13 +8305,13 @@
       <c r="A83">
         <v>3</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B83" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="C83" s="12">
+      <c r="C83" s="11">
         <v>2</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D83" s="11" t="s">
         <v>438</v>
       </c>
     </row>
@@ -8320,13 +8319,13 @@
       <c r="A84">
         <v>3</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="C84" s="12">
-        <v>1</v>
-      </c>
-      <c r="D84" s="12" t="s">
+      <c r="C84" s="11">
+        <v>1</v>
+      </c>
+      <c r="D84" s="11" t="s">
         <v>437</v>
       </c>
     </row>
@@ -8334,13 +8333,13 @@
       <c r="A85">
         <v>3</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="C85" s="12">
+      <c r="C85" s="11">
         <v>2</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="11" t="s">
         <v>439</v>
       </c>
     </row>
@@ -8348,13 +8347,13 @@
       <c r="A86">
         <v>3</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="C86" s="12">
-        <v>1</v>
-      </c>
-      <c r="D86" s="12" t="s">
+      <c r="C86" s="11">
+        <v>1</v>
+      </c>
+      <c r="D86" s="11" t="s">
         <v>433</v>
       </c>
     </row>
@@ -8362,13 +8361,13 @@
       <c r="A87">
         <v>3</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B87" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="C87" s="12">
-        <v>1</v>
-      </c>
-      <c r="D87" s="12" t="s">
+      <c r="C87" s="11">
+        <v>1</v>
+      </c>
+      <c r="D87" s="11" t="s">
         <v>436</v>
       </c>
     </row>
@@ -8376,13 +8375,13 @@
       <c r="A88">
         <v>3</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B88" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="C88" s="12">
+      <c r="C88" s="11">
         <v>2</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="11" t="s">
         <v>440</v>
       </c>
     </row>
@@ -8390,13 +8389,13 @@
       <c r="A89">
         <v>3</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="C89" s="12">
-        <v>1</v>
-      </c>
-      <c r="D89" s="12" t="s">
+      <c r="C89" s="11">
+        <v>1</v>
+      </c>
+      <c r="D89" s="11" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8404,13 +8403,13 @@
       <c r="A90">
         <v>3</v>
       </c>
-      <c r="B90" s="12" t="s">
+      <c r="B90" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="C90" s="12">
-        <v>1</v>
-      </c>
-      <c r="D90" s="12" t="s">
+      <c r="C90" s="11">
+        <v>1</v>
+      </c>
+      <c r="D90" s="11" t="s">
         <v>443</v>
       </c>
     </row>
@@ -8418,13 +8417,13 @@
       <c r="A91">
         <v>3</v>
       </c>
-      <c r="B91" s="12" t="s">
+      <c r="B91" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="C91" s="12">
+      <c r="C91" s="11">
         <v>2</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D91" s="11" t="s">
         <v>444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split datasets into groups
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D9162-31C2-498C-8E10-F24A3236A593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BF9A4A-EAD2-4968-BB10-F89A552C41D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="462">
   <si>
     <t>study</t>
   </si>
@@ -587,45 +587,21 @@
     <t>dataset3</t>
   </si>
   <si>
-    <t xml:space="preserve">Rey-Mermet (COLOR STROOP part) </t>
-  </si>
-  <si>
     <t>2000 ms</t>
   </si>
   <si>
     <t>https://raw.githubusercontent.com/jstbcs/inhibitiontasks/adding-new-data/data/mermet_2018_should/colStroop.dat.txt</t>
   </si>
   <si>
-    <t>dataset5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rey-Mermet (NUMBER STROOP part) </t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/jstbcs/inhibitiontasks/adding-new-data/data/mermet_2018_should/numStroop.dat.txt</t>
   </si>
   <si>
-    <t>dataset4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rey-Mermet (ARROW FLANKER TASK) </t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/jstbcs/inhibitiontasks/adding-new-data/data/mermet_2018_should/arrowFlanker.dat.txt</t>
   </si>
   <si>
-    <t>dataset11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rey-Mermet (LETTER FLANKER TASK) </t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/jstbcs/inhibitiontasks/adding-new-data/data/mermet_2018_should/letFlanker.dat.txt</t>
   </si>
   <si>
-    <t>dataset12</t>
-  </si>
-  <si>
     <t>https://github.com/jstbcs/inhibitiontasks/tree/adding-new-data/data/hedge_2018_reliability/Study1-Stroop</t>
   </si>
   <si>
@@ -1014,30 +990,6 @@
   </si>
   <si>
     <t>n_obs</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (COLOR STROOP part) young</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (COLOR STROOP part) old</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (NUMBER STROOP part) young</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (NUMBER STROOP part) old</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (ARROW FLANKER TASK) young</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (ARROW FLANKER TASK) old</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (LETTER FLANKER TASK) young</t>
-  </si>
-  <si>
-    <t>Rey-Mermet (LETTER FLANKER TASK) old</t>
   </si>
   <si>
     <t>Hedge study 1 stroop test</t>
@@ -1381,6 +1333,99 @@
   </si>
   <si>
     <t>Kucina, T., Wells, L., Lewis, I., De Salas, K., Kohl, A., Palmer, M. A., Sauer, J. D., Matzke, D., Aidman, E., &amp; Heathcote, A. (2023). Calibration of cognitive tests to address the reliability paradox for decision-conflict tasks. Nature Communications, 14(1). https://doi.org/10.1038/s41467-023-37777-2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (COLOR STROOP part) group 1</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (NUMBER STROOP part) Group 1</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (ARROW FLANKER TASK) Group 1</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (LETTER FLANKER TASK) Group 1</t>
+  </si>
+  <si>
+    <t>dataset12a</t>
+  </si>
+  <si>
+    <t>dataset11a</t>
+  </si>
+  <si>
+    <t>dataset4a</t>
+  </si>
+  <si>
+    <t>dataset5a</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (COLOR STROOP part) Group 2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (NUMBER STROOP part) Group 2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (ARROW FLANKER TASK) Group 2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (LETTER FLANKER TASK) Group2</t>
+  </si>
+  <si>
+    <t>dataset5b</t>
+  </si>
+  <si>
+    <t>dataset4b</t>
+  </si>
+  <si>
+    <t>dataset11b</t>
+  </si>
+  <si>
+    <t>dataset12b</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (COLOR STROOP part) young (group 1)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (NUMBER STROOP part) young (group 1)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (ARROW FLANKER TASK) young (group 1)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (LETTER FLANKER TASK) young (group 1)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (COLOR STROOP part) old (group 2)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (NUMBER STROOP part) old (group 2)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (ARROW FLANKER TASK) old (group 2)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (LETTER FLANKER TASK) old (group 2)</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (NUMBER STROOP part) group 1</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (ARROW FLANKER TASK) group 1</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (LETTER FLANKER TASK) group 1</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (COLOR STROOP part) group 2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (NUMBER STROOP part) group 2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (ARROW FLANKER TASK) group 2</t>
+  </si>
+  <si>
+    <t>Rey-Mermet (LETTER FLANKER TASK) group 2</t>
   </si>
 </sst>
 </file>
@@ -1443,7 +1488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1453,6 +1498,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1470,7 +1521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1487,9 +1538,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1807,7 +1859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2081,10 +2133,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="B11" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="C11">
         <v>2019</v>
@@ -2093,42 +2145,42 @@
         <v>32</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="G11" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="H11" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="I11" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="B12" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C12">
         <v>2023</v>
       </c>
       <c r="E12" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="G12" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="I12" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -2152,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2348,7 +2400,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2362,7 +2414,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2376,7 +2428,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2390,7 +2442,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2404,7 +2456,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2418,7 +2470,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2432,7 +2484,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2446,7 +2498,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2460,7 +2512,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2474,7 +2526,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2488,7 +2540,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2502,7 +2554,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2516,7 +2568,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2530,7 +2582,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2544,7 +2596,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2558,7 +2610,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2572,7 +2624,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2586,7 +2638,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2600,7 +2652,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2614,7 +2666,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2628,7 +2680,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2642,7 +2694,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2651,12 +2703,12 @@
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="B36">
         <v>6</v>
@@ -2665,7 +2717,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -2677,8 +2729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CF0719-54A4-4A0C-BDDA-03EA16BD7F02}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:G42"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2992,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3010,7 +3062,7 @@
         <v>98</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10">
@@ -3020,7 +3072,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3038,7 +3090,7 @@
         <v>98</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10">
@@ -3048,7 +3100,7 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3066,7 +3118,7 @@
         <v>98</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10">
@@ -3076,7 +3128,7 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3094,7 +3146,7 @@
         <v>98</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10">
@@ -3104,7 +3156,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3122,7 +3174,7 @@
         <v>98</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10">
@@ -3132,7 +3184,7 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3150,7 +3202,7 @@
         <v>98</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10">
@@ -3160,7 +3212,7 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3178,7 +3230,7 @@
         <v>98</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10">
@@ -3188,7 +3240,7 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3206,7 +3258,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10">
@@ -3216,7 +3268,7 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3234,7 +3286,7 @@
         <v>98</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10">
@@ -3244,7 +3296,7 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3259,10 +3311,10 @@
         <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10">
@@ -3272,7 +3324,7 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3290,7 +3342,7 @@
         <v>98</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10">
@@ -3300,7 +3352,7 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3318,7 +3370,7 @@
         <v>98</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10">
@@ -3328,7 +3380,7 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3346,7 +3398,7 @@
         <v>98</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10">
@@ -3356,7 +3408,7 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3374,7 +3426,7 @@
         <v>98</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10">
@@ -3384,7 +3436,7 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3399,7 +3451,7 @@
         <v>621</v>
       </c>
       <c r="G29" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -3410,7 +3462,7 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3428,7 +3480,7 @@
         <v>98</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10">
@@ -3438,7 +3490,7 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3456,7 +3508,7 @@
         <v>98</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10">
@@ -3466,7 +3518,7 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3484,7 +3536,7 @@
         <v>98</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="10">
@@ -3494,7 +3546,7 @@
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3509,10 +3561,10 @@
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="10">
@@ -3522,7 +3574,7 @@
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3540,7 +3592,7 @@
         <v>98</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -3548,7 +3600,7 @@
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3566,7 +3618,7 @@
         <v>98</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
@@ -3574,7 +3626,7 @@
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3589,7 +3641,7 @@
         <v>522</v>
       </c>
       <c r="G36" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
@@ -3598,18 +3650,18 @@
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -3618,12 +3670,12 @@
         <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -3632,12 +3684,12 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -3646,12 +3698,12 @@
         <v>31</v>
       </c>
       <c r="G40" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -3660,12 +3712,12 @@
         <v>33</v>
       </c>
       <c r="G41" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -3674,7 +3726,7 @@
         <v>30</v>
       </c>
       <c r="G42" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="S42" s="10"/>
     </row>
@@ -3706,10 +3758,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3793,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>431</v>
       </c>
       <c r="C6" t="s">
         <v>117</v>
@@ -3807,7 +3859,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
         <v>117</v>
@@ -3821,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>456</v>
       </c>
       <c r="C8" t="s">
         <v>128</v>
@@ -3835,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>457</v>
       </c>
       <c r="C9" t="s">
         <v>131</v>
@@ -4154,13 +4206,13 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="C32" t="s">
         <v>117</v>
       </c>
       <c r="D32" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -4168,13 +4220,13 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="C33" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="D33" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -4182,13 +4234,13 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="C34" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D34" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -4196,13 +4248,13 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="C35" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D35" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -4210,13 +4262,13 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="C36" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D36" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -4224,13 +4276,13 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="C37" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D37" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -4238,13 +4290,13 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C38" t="s">
         <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -4252,13 +4304,69 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="C39" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D39" t="s">
-        <v>419</v>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>458</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>459</v>
+      </c>
+      <c r="C41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>460</v>
+      </c>
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>461</v>
+      </c>
+      <c r="C43" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -4268,16 +4376,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:B61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.453125" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" customWidth="1"/>
     <col min="4" max="4" width="15.7265625" customWidth="1"/>
     <col min="7" max="7" width="13.26953125" customWidth="1"/>
@@ -4464,14 +4572,14 @@
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>182</v>
+      <c r="B6" s="13" t="s">
+        <v>431</v>
       </c>
       <c r="C6" t="s">
         <v>103</v>
       </c>
       <c r="D6">
-        <v>287</v>
+        <v>129</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -4486,27 +4594,27 @@
         <v>174</v>
       </c>
       <c r="I6" t="s">
+        <v>182</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="K6" t="s">
-        <v>185</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>186</v>
+      <c r="B7" s="13" t="s">
+        <v>432</v>
       </c>
       <c r="C7" t="s">
         <v>103</v>
       </c>
       <c r="D7">
-        <v>285</v>
+        <v>129</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -4521,27 +4629,27 @@
         <v>174</v>
       </c>
       <c r="I7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K7" t="s">
-        <v>188</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>189</v>
+      <c r="B8" s="13" t="s">
+        <v>433</v>
       </c>
       <c r="C8" t="s">
         <v>103</v>
       </c>
       <c r="D8">
-        <v>287</v>
+        <v>129</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -4556,27 +4664,27 @@
         <v>174</v>
       </c>
       <c r="I8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K8" t="s">
-        <v>191</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>192</v>
+      <c r="B9" s="13" t="s">
+        <v>434</v>
       </c>
       <c r="C9" t="s">
         <v>103</v>
       </c>
       <c r="D9">
-        <v>286</v>
+        <v>129</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -4591,13 +4699,13 @@
         <v>174</v>
       </c>
       <c r="I9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="K9" t="s">
-        <v>194</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -4629,10 +4737,10 @@
         <v>175</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K10" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -4675,10 +4783,10 @@
         <v>175</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="K11" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -4721,10 +4829,10 @@
         <v>175</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="K12" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -4767,10 +4875,10 @@
         <v>175</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -4792,7 +4900,7 @@
         <v>138</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D14">
         <v>121</v>
@@ -4813,10 +4921,10 @@
         <v>175</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="K14" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
@@ -4827,7 +4935,7 @@
         <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D15">
         <v>121</v>
@@ -4848,10 +4956,10 @@
         <v>175</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="K15" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
@@ -4859,10 +4967,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D16">
         <v>121</v>
@@ -4883,10 +4991,10 @@
         <v>175</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K16" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -4897,7 +5005,7 @@
         <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D17">
         <v>221</v>
@@ -4912,16 +5020,16 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I17" t="s">
         <v>175</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K17" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -4932,7 +5040,7 @@
         <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D18">
         <v>221</v>
@@ -4947,16 +5055,16 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I18" t="s">
         <v>175</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K18" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -4967,7 +5075,7 @@
         <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D19">
         <v>221</v>
@@ -4982,16 +5090,16 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I19" t="s">
         <v>175</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K19" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -5002,7 +5110,7 @@
         <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D20">
         <v>222</v>
@@ -5017,16 +5125,16 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I20" t="s">
         <v>175</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="K20" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -5037,7 +5145,7 @@
         <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D21">
         <v>222</v>
@@ -5052,16 +5160,16 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I21" t="s">
         <v>175</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="K21" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -5072,7 +5180,7 @@
         <v>150</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D22">
         <v>222</v>
@@ -5087,16 +5195,16 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I22" t="s">
         <v>175</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="K22" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -5107,7 +5215,7 @@
         <v>151</v>
       </c>
       <c r="C23" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D23">
         <v>222</v>
@@ -5122,16 +5230,16 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I23" t="s">
         <v>175</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K23" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -5142,7 +5250,7 @@
         <v>152</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D24">
         <v>221</v>
@@ -5157,16 +5265,16 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I24" t="s">
         <v>175</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="K24" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -5177,7 +5285,7 @@
         <v>153</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D25">
         <v>224</v>
@@ -5192,16 +5300,16 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I25" t="s">
         <v>175</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="K25" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -5209,10 +5317,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C26" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D26">
         <v>179</v>
@@ -5227,16 +5335,16 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="I26" t="s">
         <v>175</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K26" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -5265,13 +5373,13 @@
         <v>174</v>
       </c>
       <c r="I27" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="K27" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -5303,10 +5411,10 @@
         <v>175</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K28" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -5338,10 +5446,10 @@
         <v>175</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="K29" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -5366,10 +5474,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C31" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D31">
         <v>163</v>
@@ -5390,10 +5498,10 @@
         <v>175</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K31" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -5401,10 +5509,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C32" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D32">
         <v>288</v>
@@ -5425,10 +5533,10 @@
         <v>175</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K32" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -5436,10 +5544,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C33" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D33">
         <v>138</v>
@@ -5460,10 +5568,10 @@
         <v>175</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K33" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -5471,10 +5579,10 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C34" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D34">
         <v>196</v>
@@ -5495,10 +5603,10 @@
         <v>175</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K34" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -5506,10 +5614,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C35" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D35">
         <v>93</v>
@@ -5530,10 +5638,10 @@
         <v>175</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K35" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -5541,10 +5649,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D36">
         <v>177</v>
@@ -5565,10 +5673,10 @@
         <v>175</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K36" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -5576,10 +5684,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C37" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D37">
         <v>127</v>
@@ -5600,10 +5708,10 @@
         <v>175</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K37" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -5611,10 +5719,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C38" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D38">
         <v>145</v>
@@ -5635,10 +5743,10 @@
         <v>175</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K38" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -5646,10 +5754,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C39" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D39">
         <v>132</v>
@@ -5670,10 +5778,10 @@
         <v>175</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K39" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -5681,10 +5789,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C40" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D40">
         <v>82</v>
@@ -5705,10 +5813,10 @@
         <v>175</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K40" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -5716,10 +5824,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C41" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D41">
         <v>101</v>
@@ -5740,10 +5848,10 @@
         <v>175</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K41" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -5751,10 +5859,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C42" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D42">
         <v>119</v>
@@ -5775,10 +5883,10 @@
         <v>175</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K42" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -5786,10 +5894,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C43" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D43">
         <v>101</v>
@@ -5810,10 +5918,10 @@
         <v>175</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K43" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -5821,10 +5929,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C44" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D44">
         <v>120</v>
@@ -5845,10 +5953,10 @@
         <v>175</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K44" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
@@ -5856,10 +5964,10 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C45" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D45">
         <v>621</v>
@@ -5880,10 +5988,10 @@
         <v>175</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K45" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -5891,10 +5999,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C46" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D46">
         <v>97</v>
@@ -5915,10 +6023,10 @@
         <v>175</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K46" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
@@ -5926,10 +6034,10 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C47" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D47">
         <v>181</v>
@@ -5950,10 +6058,10 @@
         <v>175</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K47" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
@@ -5961,10 +6069,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C48" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D48">
         <v>84</v>
@@ -5985,10 +6093,10 @@
         <v>175</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K48" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
@@ -5996,10 +6104,10 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C49" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D49">
         <v>51</v>
@@ -6020,10 +6128,10 @@
         <v>175</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K49" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
@@ -6031,10 +6139,10 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C50" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D50">
         <v>252</v>
@@ -6055,10 +6163,10 @@
         <v>175</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K50" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
@@ -6066,10 +6174,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C51" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D51">
         <v>129</v>
@@ -6090,10 +6198,10 @@
         <v>175</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K51" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
@@ -6101,7 +6209,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="C52" t="s">
         <v>103</v>
@@ -6125,10 +6233,10 @@
         <v>175</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="K52" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
@@ -6136,10 +6244,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="C53" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="D53">
         <v>522</v>
@@ -6160,10 +6268,10 @@
         <v>175</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="K53" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
@@ -6171,7 +6279,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
@@ -6179,7 +6287,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -6187,10 +6295,10 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="C56" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D56" t="s">
         <v>104</v>
@@ -6199,13 +6307,13 @@
         <v>103</v>
       </c>
       <c r="I56" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="K56" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
@@ -6213,10 +6321,10 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="C57" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D57">
         <v>31</v>
@@ -6234,13 +6342,13 @@
         <v>103</v>
       </c>
       <c r="I57" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="K57" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
@@ -6248,10 +6356,10 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="C58" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D58">
         <v>30</v>
@@ -6269,13 +6377,13 @@
         <v>103</v>
       </c>
       <c r="I58" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="K58" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
@@ -6283,10 +6391,10 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="C59" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D59">
         <v>31</v>
@@ -6304,13 +6412,13 @@
         <v>103</v>
       </c>
       <c r="I59" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="K59" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
@@ -6318,10 +6426,10 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C60" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D60">
         <v>33</v>
@@ -6339,13 +6447,13 @@
         <v>103</v>
       </c>
       <c r="I60" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="K60" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
@@ -6353,10 +6461,10 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="C61" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="D61">
         <v>30</v>
@@ -6374,13 +6482,153 @@
         <v>103</v>
       </c>
       <c r="I61" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="K61" t="s">
-        <v>427</v>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>439</v>
+      </c>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62">
+        <v>158</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <v>74</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>174</v>
+      </c>
+      <c r="I62" t="s">
+        <v>182</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="K62" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>440</v>
+      </c>
+      <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63">
+        <v>156</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <v>74</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>174</v>
+      </c>
+      <c r="I63" t="s">
+        <v>182</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K63" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>441</v>
+      </c>
+      <c r="C64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64">
+        <v>158</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>74</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>174</v>
+      </c>
+      <c r="I64" t="s">
+        <v>182</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K64" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>442</v>
+      </c>
+      <c r="C65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65">
+        <v>157</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>74</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>174</v>
+      </c>
+      <c r="I65" t="s">
+        <v>182</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K65" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -6442,6 +6690,10 @@
     <hyperlink ref="J59" r:id="rId55" xr:uid="{CE4B6D3A-CEF7-44CB-AC73-740F7CFC5E01}"/>
     <hyperlink ref="J60" r:id="rId56" xr:uid="{992FA71F-3DB4-4C96-AB9E-13D6BE604AAC}"/>
     <hyperlink ref="J61" r:id="rId57" xr:uid="{DA7FE050-E207-4231-B433-4E90CAB92A1A}"/>
+    <hyperlink ref="J62" r:id="rId58" xr:uid="{1576BAA7-96DE-41FC-9924-1E9FDC6C95E8}"/>
+    <hyperlink ref="J63" r:id="rId59" xr:uid="{C9D15297-2947-4FFF-A390-BC4C5EC649E5}"/>
+    <hyperlink ref="J64" r:id="rId60" xr:uid="{34E07ECA-2FE3-4B63-B4DE-0BE259FBAC27}"/>
+    <hyperlink ref="J65" r:id="rId61" xr:uid="{9543C0EC-B435-47CE-9D9A-F88D908304C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6449,10 +6701,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73:B82"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6467,13 +6719,13 @@
         <v>163</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -6487,7 +6739,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -6501,7 +6753,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -6515,7 +6767,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -6529,7 +6781,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -6543,7 +6795,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -6557,7 +6809,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -6571,7 +6823,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -6585,7 +6837,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -6599,7 +6851,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -6613,7 +6865,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -6627,7 +6879,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -6641,7 +6893,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -6655,7 +6907,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -6669,7 +6921,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -6683,7 +6935,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -6697,7 +6949,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -6711,7 +6963,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -6725,7 +6977,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -6739,7 +6991,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -6753,7 +7005,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -6767,7 +7019,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -6781,7 +7033,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -6795,7 +7047,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -6809,7 +7061,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -6823,7 +7075,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -6837,7 +7089,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -6851,7 +7103,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -6865,7 +7117,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -6873,13 +7125,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -6887,13 +7139,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -6901,13 +7153,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -6915,13 +7167,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -6929,13 +7181,13 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C34">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -6943,13 +7195,13 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -6957,13 +7209,13 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C36">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -6971,13 +7223,13 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C37">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -6985,13 +7237,13 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C38">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -6999,13 +7251,13 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C39">
         <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -7013,13 +7265,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C40">
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -7027,13 +7279,13 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C41">
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -7041,13 +7293,13 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C42">
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -7055,13 +7307,13 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C43">
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -7075,7 +7327,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -7089,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -7103,7 +7355,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -7120,13 +7372,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -7134,13 +7386,13 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -7148,13 +7400,13 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -7162,13 +7414,13 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -7176,13 +7428,13 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -7190,13 +7442,13 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -7204,13 +7456,13 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -7218,13 +7470,13 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -7232,13 +7484,13 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -7246,13 +7498,13 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -7260,13 +7512,13 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -7274,13 +7526,13 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -7288,13 +7540,13 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -7302,13 +7554,13 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -7316,13 +7568,13 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -7330,13 +7582,13 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -7344,13 +7596,13 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -7358,13 +7610,13 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -7372,13 +7624,13 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -7386,13 +7638,13 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -7400,13 +7652,13 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -7414,13 +7666,13 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7428,13 +7680,13 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C70">
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -7442,13 +7694,13 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -7456,123 +7708,167 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="C72">
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="C74">
         <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="C76">
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="C79">
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="C82">
         <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>444</v>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>439</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>440</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>441</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>442</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -7584,8 +7880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7601,19 +7897,19 @@
         <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -7653,7 +7949,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -7661,7 +7957,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>326</v>
+        <v>451</v>
       </c>
       <c r="E7" s="9"/>
     </row>
@@ -7670,7 +7966,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>327</v>
+        <v>448</v>
       </c>
       <c r="E8" s="9"/>
     </row>
@@ -7679,7 +7975,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>328</v>
+        <v>452</v>
       </c>
       <c r="E9" s="9"/>
     </row>
@@ -7688,7 +7984,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>329</v>
+        <v>449</v>
       </c>
       <c r="E10" s="9"/>
     </row>
@@ -7697,7 +7993,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>330</v>
+        <v>453</v>
       </c>
       <c r="E11" s="9"/>
     </row>
@@ -7706,7 +8002,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>331</v>
+        <v>450</v>
       </c>
       <c r="E12" s="9"/>
     </row>
@@ -7715,7 +8011,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>332</v>
+        <v>454</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -7724,7 +8020,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -7732,7 +8028,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -7740,7 +8036,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -7748,7 +8044,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -7756,7 +8052,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -7764,7 +8060,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -7772,7 +8068,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -7780,7 +8076,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -7796,7 +8092,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -7804,7 +8100,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -7884,7 +8180,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -7892,7 +8188,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -7900,7 +8196,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -7908,7 +8204,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -7916,7 +8212,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -7924,7 +8220,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -7932,7 +8228,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -7940,7 +8236,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -7948,7 +8244,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -7956,7 +8252,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -7964,7 +8260,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -7972,7 +8268,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -7980,7 +8276,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -7988,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -8028,7 +8324,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -8036,7 +8332,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -8044,7 +8340,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -8052,7 +8348,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -8060,7 +8356,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -8068,7 +8364,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -8076,7 +8372,7 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -8084,7 +8380,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -8092,7 +8388,7 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -8100,7 +8396,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -8108,7 +8404,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -8116,7 +8412,7 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -8124,7 +8420,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -8132,7 +8428,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -8140,7 +8436,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -8148,7 +8444,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -8156,7 +8452,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -8164,7 +8460,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -8172,7 +8468,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -8180,7 +8476,7 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -8188,7 +8484,7 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -8196,7 +8492,7 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -8204,7 +8500,7 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -8212,7 +8508,7 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
@@ -8220,7 +8516,7 @@
         <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -8228,7 +8524,7 @@
         <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -8236,13 +8532,13 @@
         <v>3</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C78" s="11">
         <v>1</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -8250,13 +8546,13 @@
         <v>3</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C79" s="11">
         <v>2</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -8264,13 +8560,13 @@
         <v>3</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="C80" s="11">
         <v>1</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -8278,13 +8574,13 @@
         <v>3</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="C81" s="11">
         <v>2</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -8292,13 +8588,13 @@
         <v>3</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="C82" s="11">
         <v>1</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
@@ -8306,13 +8602,13 @@
         <v>3</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="C83" s="11">
         <v>2</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
@@ -8320,13 +8616,13 @@
         <v>3</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="C84" s="11">
         <v>1</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
@@ -8334,13 +8630,13 @@
         <v>3</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="C85" s="11">
         <v>2</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
@@ -8348,13 +8644,13 @@
         <v>3</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="C86" s="11">
         <v>1</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
@@ -8362,13 +8658,13 @@
         <v>3</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="C87" s="11">
         <v>1</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
@@ -8376,13 +8672,13 @@
         <v>3</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="C88" s="11">
         <v>2</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
@@ -8390,13 +8686,13 @@
         <v>3</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C89" s="11">
         <v>1</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
@@ -8404,13 +8700,13 @@
         <v>3</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="C90" s="11">
         <v>1</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
@@ -8418,13 +8714,13 @@
         <v>3</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="C91" s="11">
         <v>2</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add loeffler list object
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D574C7-B710-41AB-B4FF-59198CB12E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EFDAE6-7EB0-45F7-8FAD-DA8CE5DCECDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="488">
   <si>
     <t>study</t>
   </si>
@@ -1479,10 +1479,31 @@
     <t>dataset59</t>
   </si>
   <si>
-    <t xml:space="preserve">Löffler stroop </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2? </t>
+    <t>Löffler stroop</t>
+  </si>
+  <si>
+    <t>Löffler negative priming</t>
+  </si>
+  <si>
+    <t>Löffler flanker</t>
+  </si>
+  <si>
+    <t>https://github.com/jstbcs/acdc-database/tree/main/data/loeffler_2022_common/Stroop_task</t>
+  </si>
+  <si>
+    <t>https://github.com/jstbcs/acdc-database/tree/main/data/loeffler_2022_common/Flanker_task</t>
+  </si>
+  <si>
+    <t>dataset61</t>
+  </si>
+  <si>
+    <t>https://github.com/jstbcs/acdc-database/tree/main/data/loeffler_2022_common/Neg_priming_task</t>
+  </si>
+  <si>
+    <t>Löffler, C., Frischkorn, G. T., Hagemann, D., Sadus, K., &amp; Schubert, A. L. (2022). The common factor of executive functions measures nothing but speed of information uptake.  PsyArXiv. https://doi.org/10.31234/osf.io/xvdyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In each trial an O and an X appeared, each on either side of the screen. Participants had to classify the position of the O while ignoring the X. In negatively primed trials (incongruent), the O appeared on the side that the X had appeared in the previous trials. Trials in which the O appeared on the same side as it had in the previous trial, no negative priming occured (congruent). </t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1599,6 +1620,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1917,7 +1939,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2259,8 +2281,8 @@
       <c r="G13" t="s">
         <v>466</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>104</v>
+      <c r="H13" s="14" t="s">
+        <v>486</v>
       </c>
       <c r="I13" t="s">
         <v>465</v>
@@ -2827,7 +2849,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3875,8 +3897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="D33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4513,6 +4535,9 @@
       <c r="C46" t="s">
         <v>472</v>
       </c>
+      <c r="D46" t="s">
+        <v>487</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4521,10 +4546,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6777,17 +6802,23 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>1</v>
+      </c>
       <c r="B66" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C66" t="s">
         <v>103</v>
       </c>
+      <c r="D66">
+        <v>148</v>
+      </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -6795,22 +6826,34 @@
       <c r="H66" t="s">
         <v>103</v>
       </c>
+      <c r="I66" t="s">
+        <v>175</v>
+      </c>
+      <c r="J66" t="s">
+        <v>483</v>
+      </c>
       <c r="K66" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>1</v>
+      </c>
       <c r="B67" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C67" t="s">
         <v>103</v>
       </c>
+      <c r="D67">
+        <v>147</v>
+      </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -6818,8 +6861,49 @@
       <c r="H67" t="s">
         <v>103</v>
       </c>
+      <c r="I67" t="s">
+        <v>175</v>
+      </c>
+      <c r="J67" t="s">
+        <v>482</v>
+      </c>
       <c r="K67" t="s">
-        <v>478</v>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>480</v>
+      </c>
+      <c r="C68" t="s">
+        <v>364</v>
+      </c>
+      <c r="D68">
+        <v>142</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>192</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68" t="s">
+        <v>103</v>
+      </c>
+      <c r="I68" t="s">
+        <v>175</v>
+      </c>
+      <c r="J68" t="s">
+        <v>485</v>
+      </c>
+      <c r="K68" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -6892,10 +6976,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8064,18 +8148,35 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C87">
         <v>1</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>479</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
         <v>480</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -8085,10 +8186,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8930,6 +9031,21 @@
         <v>428</v>
       </c>
     </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B92" s="11" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B93" s="11" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B94" s="11" t="s">
+        <v>480</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added metadata for Robinson paper
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EFDAE6-7EB0-45F7-8FAD-DA8CE5DCECDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF5CC48-2CE5-467F-8F94-43CA2BF2618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="504">
   <si>
     <t>study</t>
   </si>
@@ -1504,6 +1504,54 @@
   </si>
   <si>
     <t xml:space="preserve">In each trial an O and an X appeared, each on either side of the screen. Participants had to classify the position of the O while ignoring the X. In negatively primed trials (incongruent), the O appeared on the side that the X had appeared in the previous trials. Trials in which the O appeared on the same side as it had in the previous trial, no negative priming occured (congruent). </t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>500?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robinson Flanker task </t>
+  </si>
+  <si>
+    <t>Arrow flanker task in which participants idnicate the direction of a central arrow while ignoring the direction of flanking arrows (one left, one right, one below, and one above the central arrow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robinson flanker </t>
+  </si>
+  <si>
+    <t>dataset62</t>
+  </si>
+  <si>
+    <t>Robinson flanker</t>
+  </si>
+  <si>
+    <t>Users of the Lumosity platform who had trained at least 60 sessions (of 60 trails each) of the task switching and flanker task</t>
+  </si>
+  <si>
+    <t>60?</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This study links computational models of the task switching and the Erikson flanker task, to determining which latent constructs are shared between cognitive control tasks. Data is taken from users of an online platform who extensively trained for the tasks. </t>
+  </si>
+  <si>
+    <t>Maria M. Robinson, Mark Steyvers</t>
+  </si>
+  <si>
+    <t>Robinson, M. M., &amp; Steyvers, M. (2023). Linking computational models of two core tasks of cognitive control. Psychological Review, 130(1), 71–101.https://doi.org/10.1037/rev0000395</t>
+  </si>
+  <si>
+    <t>robinson_2023_linking</t>
+  </si>
+  <si>
+    <t>theories of cognitive control, linking models of cognition, Eriksen flanker task, task-switching task, cognitive training</t>
+  </si>
+  <si>
+    <t>mrobinson@ucsd.edu</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1561,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1561,6 +1609,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1620,7 +1675,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1936,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2281,11 +2336,37 @@
       <c r="G13" t="s">
         <v>466</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" t="s">
         <v>486</v>
       </c>
       <c r="I13" t="s">
         <v>465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>488</v>
+      </c>
+      <c r="B14" t="s">
+        <v>499</v>
+      </c>
+      <c r="C14">
+        <v>2023</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>503</v>
+      </c>
+      <c r="G14" t="s">
+        <v>502</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="I14" t="s">
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -2300,6 +2381,7 @@
     <hyperlink ref="F5" r:id="rId8" xr:uid="{1AC344C5-7FEF-42ED-A7EA-742769BFDA83}"/>
     <hyperlink ref="F11" r:id="rId9" xr:uid="{6EE7083C-CB23-46FC-B9FB-ED39AD2DCC15}"/>
     <hyperlink ref="F12" r:id="rId10" xr:uid="{E1360CE3-FFB6-477F-A262-E234B0E97B60}"/>
+    <hyperlink ref="H14" r:id="rId11" display="https://psycnet.apa.org/doi/10.1037/rev0000395" xr:uid="{5AC0FBBB-6C20-48BE-BC60-DBCC282D7CF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2307,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2839,6 +2921,20 @@
         <v>467</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>488</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>498</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2848,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CF0719-54A4-4A0C-BDDA-03EA16BD7F02}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3871,6 +3967,24 @@
       <c r="S43" s="10"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>488</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>58</v>
+      </c>
+      <c r="E44">
+        <v>0.66</v>
+      </c>
+      <c r="F44" t="s">
+        <v>489</v>
+      </c>
+      <c r="G44" t="s">
+        <v>495</v>
+      </c>
       <c r="P44" s="10"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.35">
@@ -3895,10 +4009,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="D33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4539,6 +4653,17 @@
         <v>487</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>490</v>
+      </c>
+      <c r="C47" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" t="s">
+        <v>491</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4546,10 +4671,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V68"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6904,6 +7029,32 @@
       </c>
       <c r="K68" t="s">
         <v>484</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>492</v>
+      </c>
+      <c r="C69" t="s">
+        <v>364</v>
+      </c>
+      <c r="E69" t="s">
+        <v>496</v>
+      </c>
+      <c r="F69">
+        <v>60</v>
+      </c>
+      <c r="H69" t="s">
+        <v>103</v>
+      </c>
+      <c r="I69" t="s">
+        <v>412</v>
+      </c>
+      <c r="J69" t="s">
+        <v>497</v>
+      </c>
+      <c r="K69" t="s">
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -6976,10 +7127,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8179,6 +8330,17 @@
         <v>281</v>
       </c>
     </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>494</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8186,10 +8348,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92:B94"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9046,6 +9208,11 @@
         <v>480</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B95" s="11" t="s">
+        <v>494</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code & metainfo for enkavi shape matching
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF5CC48-2CE5-467F-8F94-43CA2BF2618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F232D2-ECF2-4E47-9DFB-A5172B5839F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="509">
   <si>
     <t>study</t>
   </si>
@@ -1552,6 +1552,21 @@
   </si>
   <si>
     <t>mrobinson@ucsd.edu</t>
+  </si>
+  <si>
+    <t>Enkavi shape matching</t>
+  </si>
+  <si>
+    <t>Enakvi shape matching task</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/jstbcs/acdc-database/main/data/enkavi_2019_large/shape_matching.csv</t>
+  </si>
+  <si>
+    <t>dataset63</t>
+  </si>
+  <si>
+    <t>Participants had to indicate whether a green and a white shape, appearing on opposite sides of the screen, were identical. On half of the trials, a distracting red shape appeared underneath the green one. Participants had to ignore the red shape. Negative priming occurs when the current target shape (green) is identical to the distractor (red shape) in the previous trial. In our data base, such trials are coded as incongruent.</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2009,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2391,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4009,10 +4024,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4664,6 +4679,17 @@
         <v>491</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>504</v>
+      </c>
+      <c r="C48" t="s">
+        <v>396</v>
+      </c>
+      <c r="D48" t="s">
+        <v>508</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4671,10 +4697,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V69"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7038,7 +7064,8 @@
       <c r="C69" t="s">
         <v>364</v>
       </c>
-      <c r="E69" t="s">
+      <c r="D69" s="13"/>
+      <c r="E69" s="13" t="s">
         <v>496</v>
       </c>
       <c r="F69">
@@ -7050,11 +7077,40 @@
       <c r="I69" t="s">
         <v>412</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J69" s="13" t="s">
         <v>497</v>
       </c>
       <c r="K69" t="s">
         <v>493</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>505</v>
+      </c>
+      <c r="C70" t="s">
+        <v>364</v>
+      </c>
+      <c r="D70">
+        <v>522</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>180</v>
+      </c>
+      <c r="H70" t="s">
+        <v>103</v>
+      </c>
+      <c r="I70" t="s">
+        <v>175</v>
+      </c>
+      <c r="J70" t="s">
+        <v>506</v>
+      </c>
+      <c r="K70" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add code for enkavi shape matching task
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F232D2-ECF2-4E47-9DFB-A5172B5839F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8E3053-F382-40C4-BE68-C509E82AE175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="497">
   <si>
     <t>study</t>
   </si>
@@ -1506,54 +1506,12 @@
     <t xml:space="preserve">In each trial an O and an X appeared, each on either side of the screen. Participants had to classify the position of the O while ignoring the X. In negatively primed trials (incongruent), the O appeared on the side that the X had appeared in the previous trials. Trials in which the O appeared on the same side as it had in the previous trial, no negative priming occured (congruent). </t>
   </si>
   <si>
-    <t>Robinson</t>
-  </si>
-  <si>
-    <t>500?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robinson Flanker task </t>
-  </si>
-  <si>
-    <t>Arrow flanker task in which participants idnicate the direction of a central arrow while ignoring the direction of flanking arrows (one left, one right, one below, and one above the central arrow)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robinson flanker </t>
-  </si>
-  <si>
     <t>dataset62</t>
   </si>
   <si>
     <t>Robinson flanker</t>
   </si>
   <si>
-    <t>Users of the Lumosity platform who had trained at least 60 sessions (of 60 trails each) of the task switching and flanker task</t>
-  </si>
-  <si>
-    <t>60?</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This study links computational models of the task switching and the Erikson flanker task, to determining which latent constructs are shared between cognitive control tasks. Data is taken from users of an online platform who extensively trained for the tasks. </t>
-  </si>
-  <si>
-    <t>Maria M. Robinson, Mark Steyvers</t>
-  </si>
-  <si>
-    <t>Robinson, M. M., &amp; Steyvers, M. (2023). Linking computational models of two core tasks of cognitive control. Psychological Review, 130(1), 71–101.https://doi.org/10.1037/rev0000395</t>
-  </si>
-  <si>
-    <t>robinson_2023_linking</t>
-  </si>
-  <si>
-    <t>theories of cognitive control, linking models of cognition, Eriksen flanker task, task-switching task, cognitive training</t>
-  </si>
-  <si>
-    <t>mrobinson@ucsd.edu</t>
-  </si>
-  <si>
     <t>Enkavi shape matching</t>
   </si>
   <si>
@@ -1563,10 +1521,16 @@
     <t>https://raw.githubusercontent.com/jstbcs/acdc-database/main/data/enkavi_2019_large/shape_matching.csv</t>
   </si>
   <si>
-    <t>dataset63</t>
-  </si>
-  <si>
     <t>Participants had to indicate whether a green and a white shape, appearing on opposite sides of the screen, were identical. On half of the trials, a distracting red shape appeared underneath the green one. Participants had to ignore the red shape. Negative priming occurs when the current target shape (green) is identical to the distractor (red shape) in the previous trial. In our data base, such trials are coded as incongruent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkavi shape matching task </t>
+  </si>
+  <si>
+    <t>Enkavi shape matching task</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1691,6 +1655,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2009,7 +1977,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A14" sqref="A14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2359,30 +2327,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>488</v>
-      </c>
-      <c r="B14" t="s">
-        <v>499</v>
-      </c>
-      <c r="C14">
-        <v>2023</v>
-      </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" t="s">
-        <v>503</v>
-      </c>
-      <c r="G14" t="s">
-        <v>502</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>500</v>
-      </c>
-      <c r="I14" t="s">
-        <v>501</v>
-      </c>
+      <c r="H14" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2396,7 +2341,6 @@
     <hyperlink ref="F5" r:id="rId8" xr:uid="{1AC344C5-7FEF-42ED-A7EA-742769BFDA83}"/>
     <hyperlink ref="F11" r:id="rId9" xr:uid="{6EE7083C-CB23-46FC-B9FB-ED39AD2DCC15}"/>
     <hyperlink ref="F12" r:id="rId10" xr:uid="{E1360CE3-FFB6-477F-A262-E234B0E97B60}"/>
-    <hyperlink ref="H14" r:id="rId11" display="https://psycnet.apa.org/doi/10.1037/rev0000395" xr:uid="{5AC0FBBB-6C20-48BE-BC60-DBCC282D7CF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2404,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A38" sqref="A38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2936,20 +2880,6 @@
         <v>467</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>488</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>498</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2960,7 +2890,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="B44" sqref="B44:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3982,24 +3912,6 @@
       <c r="S43" s="10"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>488</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>58</v>
-      </c>
-      <c r="E44">
-        <v>0.66</v>
-      </c>
-      <c r="F44" t="s">
-        <v>489</v>
-      </c>
-      <c r="G44" t="s">
-        <v>495</v>
-      </c>
       <c r="P44" s="10"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.35">
@@ -4024,10 +3936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4673,21 +4585,10 @@
         <v>490</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>396</v>
       </c>
       <c r="D47" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>504</v>
-      </c>
-      <c r="C48" t="s">
-        <v>396</v>
-      </c>
-      <c r="D48" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -4697,10 +4598,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7059,58 +6960,34 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C69" t="s">
         <v>364</v>
       </c>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13" t="s">
-        <v>496</v>
+      <c r="D69">
+        <v>522</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
       </c>
       <c r="F69">
-        <v>60</v>
+        <v>180</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
       </c>
       <c r="H69" t="s">
         <v>103</v>
       </c>
       <c r="I69" t="s">
-        <v>412</v>
-      </c>
-      <c r="J69" s="13" t="s">
-        <v>497</v>
+        <v>175</v>
+      </c>
+      <c r="J69" t="s">
+        <v>492</v>
       </c>
       <c r="K69" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
-        <v>505</v>
-      </c>
-      <c r="C70" t="s">
-        <v>364</v>
-      </c>
-      <c r="D70">
-        <v>522</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>180</v>
-      </c>
-      <c r="H70" t="s">
-        <v>103</v>
-      </c>
-      <c r="I70" t="s">
-        <v>175</v>
-      </c>
-      <c r="J70" t="s">
-        <v>506</v>
-      </c>
-      <c r="K70" t="s">
-        <v>507</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -7185,8 +7062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8390,12 +8267,8 @@
       <c r="B90" t="s">
         <v>494</v>
       </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>281</v>
-      </c>
+      <c r="C90" s="15"/>
+      <c r="D90" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8404,10 +8277,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1346955-E561-4BA2-96D5-97F4D829E993}">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9266,7 +9139,17 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B95" s="11" t="s">
-        <v>494</v>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B96" s="11" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="13" t="s">
+        <v>496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added enkavi shape matching retest data
</commit_message>
<xml_diff>
--- a/Create_db/add_data/Book.xlsx
+++ b/Create_db/add_data/Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\acdc-database\Create_db\add_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8E3053-F382-40C4-BE68-C509E82AE175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A17529-217D-4C82-A20E-993494BFE08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8270" yWindow="21490" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_table" sheetId="1" r:id="rId1"/>
@@ -1521,9 +1521,6 @@
     <t>https://raw.githubusercontent.com/jstbcs/acdc-database/main/data/enkavi_2019_large/shape_matching.csv</t>
   </si>
   <si>
-    <t>Participants had to indicate whether a green and a white shape, appearing on opposite sides of the screen, were identical. On half of the trials, a distracting red shape appeared underneath the green one. Participants had to ignore the red shape. Negative priming occurs when the current target shape (green) is identical to the distractor (red shape) in the previous trial. In our data base, such trials are coded as incongruent.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enkavi shape matching task </t>
   </si>
   <si>
@@ -1531,6 +1528,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants had to indicate whether a green and a white shape, appearing on opposite sides of the screen, were identical. On half of the trials, a distracting red shape appeared underneath the green one. Participants had to ignore the red shape. Negative priming occurs when the current probe shape (green) is identical to the distractor (red shape) in the previous trial. In our data base, such trials are coded as incongruent. Trials in which the red shape and the green shape were not identical are coded as congruent, and trials where there had been no distractor in the previous trial are neutral. </t>
   </si>
 </sst>
 </file>
@@ -1633,7 +1633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1655,8 +1655,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1977,7 +1976,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2350,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56954744-AC6A-40FE-AAFF-6494252F15D0}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:D38"/>
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2890,7 +2889,7 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:J44"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3938,8 +3937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE889DDA-04E7-4061-88E6-E2249FD9EC36}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:D47"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4588,7 +4587,7 @@
         <v>396</v>
       </c>
       <c r="D47" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -4600,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899529-D1A8-430F-A7D5-5D9280DFB08C}">
   <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6959,6 +6958,9 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>1</v>
+      </c>
       <c r="B69" t="s">
         <v>491</v>
       </c>
@@ -6981,7 +6983,7 @@
         <v>103</v>
       </c>
       <c r="I69" t="s">
-        <v>175</v>
+        <v>103</v>
       </c>
       <c r="J69" t="s">
         <v>492</v>
@@ -7062,8 +7064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8BAC05-7681-45EF-A477-0E81CBAC477D}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90:D90"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8265,10 +8267,10 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>494</v>
-      </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="16"/>
+        <v>493</v>
+      </c>
+      <c r="C90" s="13"/>
+      <c r="D90" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9144,12 +9146,12 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B96" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" s="13" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>